<commit_message>
identified not usable points
Highlighted the discussion points.
</commit_message>
<xml_diff>
--- a/Project Management/CHKL_PLNREV.xlsx
+++ b/Project Management/CHKL_PLNREV.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="15480" windowHeight="8445" activeTab="1"/>
@@ -164,8 +164,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,8 +196,16 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +215,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF4F81BD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,7 +286,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -295,6 +309,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -302,7 +328,7 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -321,7 +347,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -340,7 +366,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -357,7 +383,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -384,7 +410,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -408,7 +434,7 @@
           <bgColor rgb="FF4F81BD"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -508,6 +534,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -542,6 +569,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -717,26 +745,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="22.5">
+    <row r="1" spans="1:1" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="22.5">
+    <row r="4" spans="1:1" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>42</v>
       </c>
@@ -747,14 +775,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="8" customWidth="1"/>
     <col min="2" max="2" width="40.28515625" customWidth="1"/>
@@ -762,7 +790,7 @@
     <col min="4" max="4" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="22.5">
+    <row r="2" spans="1:7" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
@@ -773,27 +801,27 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="4" spans="1:7" ht="16.5">
+    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16.5">
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16.5">
+    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16.5">
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -807,37 +835,37 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="45">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="30">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>3</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="30">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -847,7 +875,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" ht="30">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>5</v>
       </c>
@@ -857,17 +885,17 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" ht="45">
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>6</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" ht="45">
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>7</v>
       </c>
@@ -877,7 +905,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" ht="90">
+    <row r="20" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>8</v>
       </c>
@@ -887,7 +915,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" ht="30">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>9</v>
       </c>
@@ -897,7 +925,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" ht="45">
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>10</v>
       </c>
@@ -907,7 +935,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" ht="45">
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>11</v>
       </c>
@@ -917,7 +945,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" ht="35.25" customHeight="1">
+    <row r="24" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>12</v>
       </c>
@@ -927,7 +955,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" ht="30">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>13</v>
       </c>
@@ -937,7 +965,7 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" ht="30">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>14</v>
       </c>
@@ -947,7 +975,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" ht="30">
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>15</v>
       </c>
@@ -957,7 +985,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" ht="30">
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>16</v>
       </c>
@@ -967,7 +995,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>17</v>
       </c>
@@ -977,7 +1005,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" ht="30">
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>18</v>
       </c>
@@ -987,7 +1015,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" ht="30">
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>19</v>
       </c>
@@ -997,7 +1025,7 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" ht="30">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>20</v>
       </c>
@@ -1007,7 +1035,7 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" ht="30">
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>21</v>
       </c>
@@ -1017,7 +1045,7 @@
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" ht="30">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>22</v>
       </c>
@@ -1027,7 +1055,7 @@
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" ht="45">
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>23</v>
       </c>
@@ -1037,7 +1065,7 @@
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" ht="30">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>24</v>
       </c>
@@ -1047,7 +1075,7 @@
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" ht="45">
+    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>25</v>
       </c>
@@ -1057,7 +1085,7 @@
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" ht="30">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>26</v>
       </c>
@@ -1067,7 +1095,7 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>27</v>
       </c>
@@ -1077,7 +1105,7 @@
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>28</v>
       </c>
@@ -1087,7 +1115,7 @@
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" ht="30">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>29</v>
       </c>
@@ -1097,7 +1125,7 @@
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" ht="45">
+    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>30</v>
       </c>
@@ -1107,7 +1135,7 @@
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" ht="30">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>31</v>
       </c>
@@ -1117,7 +1145,7 @@
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" ht="30">
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>32</v>
       </c>
@@ -1127,7 +1155,7 @@
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" ht="30">
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>33</v>
       </c>
@@ -1137,27 +1165,27 @@
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>34</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="12" t="s">
         <v>40</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>35</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="13" t="s">
         <v>36</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>36</v>
       </c>
@@ -1167,7 +1195,7 @@
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="1:4" ht="30">
+    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>37</v>
       </c>
@@ -1195,6 +1223,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005A068604E74C047BC66B3ED07869872" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7d65b694ac3f1c289d6201da35c196e2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -1243,32 +1286,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E6F5A04-C6BC-4BC3-8CB0-447E3C344A6D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1FE17C5-771B-4F44-9535-2FC09B1C82EC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1282,15 +1309,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1FE17C5-771B-4F44-9535-2FC09B1C82EC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E6F5A04-C6BC-4BC3-8CB0-447E3C344A6D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
review points discussed and un-highlighted.
</commit_message>
<xml_diff>
--- a/Project Management/CHKL_PLNREV.xlsx
+++ b/Project Management/CHKL_PLNREV.xlsx
@@ -125,9 +125,6 @@
     <t>Have the DAR activities been identified and stated clearly?</t>
   </si>
   <si>
-    <t>Has the R&amp;R matrix been filled?</t>
-  </si>
-  <si>
     <t>Is the version of the template used current?</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>Is the product development lifecycle appropriate? Has it been referred from defined project lifecycle?</t>
+  </si>
+  <si>
+    <t>Has the team been identified?</t>
   </si>
 </sst>
 </file>
@@ -205,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,12 +215,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF4F81BD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -306,19 +300,19 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -749,7 +743,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,12 +755,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -779,7 +773,7 @@
   <dimension ref="A2:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,15 +785,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -839,7 +833,7 @@
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="1"/>
@@ -849,7 +843,7 @@
       <c r="A14" s="1">
         <v>2</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="1"/>
@@ -859,8 +853,8 @@
       <c r="A15" s="1">
         <v>3</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>37</v>
+      <c r="B15" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -889,7 +883,7 @@
       <c r="A18" s="1">
         <v>6</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="1"/>
@@ -900,7 +894,7 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -940,7 +934,7 @@
         <v>11</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -970,7 +964,7 @@
         <v>14</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -980,7 +974,7 @@
         <v>15</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1050,7 +1044,7 @@
         <v>22</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -1169,8 +1163,8 @@
       <c r="A46" s="1">
         <v>34</v>
       </c>
-      <c r="B46" s="12" t="s">
-        <v>40</v>
+      <c r="B46" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1180,7 +1174,7 @@
         <v>35</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -1190,7 +1184,7 @@
         <v>36</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
@@ -1200,7 +1194,7 @@
         <v>37</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
@@ -1223,21 +1217,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005A068604E74C047BC66B3ED07869872" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7d65b694ac3f1c289d6201da35c196e2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -1286,16 +1265,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1FE17C5-771B-4F44-9535-2FC09B1C82EC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E6F5A04-C6BC-4BC3-8CB0-447E3C344A6D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1309,16 +1304,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E6F5A04-C6BC-4BC3-8CB0-447E3C344A6D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1FE17C5-771B-4F44-9535-2FC09B1C82EC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
finalised plan review checklist
</commit_message>
<xml_diff>
--- a/Project Management/CHKL_PLNREV.xlsx
+++ b/Project Management/CHKL_PLNREV.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="15480" windowHeight="8445" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="15480" windowHeight="8445"/>
   </bookViews>
   <sheets>
     <sheet name="Revision History" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Project code:</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Plan Review Checklist</t>
   </si>
   <si>
-    <t>Has the table of contents been updated?</t>
-  </si>
-  <si>
-    <t>Has the template been renamed in conformance with the CM procedure?([ProjectCode_PRJPLN]</t>
-  </si>
-  <si>
     <t>Has the scope of the project been clearly identified?</t>
   </si>
   <si>
@@ -125,24 +119,15 @@
     <t>Have the DAR activities been identified and stated clearly?</t>
   </si>
   <si>
-    <t>Is the version of the template used current?</t>
-  </si>
-  <si>
     <t>Has the plan been approved?</t>
   </si>
   <si>
     <t>Has it been place under Configuration management?</t>
   </si>
   <si>
-    <t>Is the escalation section updated?</t>
-  </si>
-  <si>
     <t>have the RPN been calculated using proper risk ratings?</t>
   </si>
   <si>
-    <t>Template Version - 1</t>
-  </si>
-  <si>
     <t>Genus Innovation Limited</t>
   </si>
   <si>
@@ -159,13 +144,16 @@
   </si>
   <si>
     <t>Has the team been identified?</t>
+  </si>
+  <si>
+    <t>Template Version - 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,14 +183,6 @@
       <color rgb="FF4F81BD"/>
       <name val="Cambria"/>
       <family val="1"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -280,7 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -300,20 +280,14 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -441,8 +415,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A12:D49" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="A12:D49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A12:D45" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A12:D45"/>
   <tableColumns count="4">
     <tableColumn id="1" name="S. No" dataDxfId="3"/>
     <tableColumn id="2" name="Checkpoint" dataDxfId="2"/>
@@ -742,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,12 +729,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -770,10 +744,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G49"/>
+  <dimension ref="A2:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,47 +803,47 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>3</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>5</v>
       </c>
@@ -879,11 +853,11 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>6</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="1"/>
@@ -894,57 +868,57 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>9</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>15</v>
+      <c r="B21" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>10</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>11</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>12</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>23</v>
+      <c r="B24" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -953,18 +927,18 @@
       <c r="A25" s="1">
         <v>13</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>14</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -974,7 +948,7 @@
         <v>15</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -989,7 +963,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>17</v>
       </c>
@@ -1003,78 +977,78 @@
       <c r="A30" s="1">
         <v>18</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="B30" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>19</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>20</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="B32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>21</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>22</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>23</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>24</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>25</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -1084,27 +1058,27 @@
         <v>26</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>27</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>28</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -1114,32 +1088,32 @@
         <v>29</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>30</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>31</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>33</v>
+      <c r="B43" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>32</v>
       </c>
@@ -1158,53 +1132,13 @@
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>34</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>35</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>36</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-    </row>
-    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>37</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:C49">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:C45">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>